<commit_message>
change `oa` to `ao`
Change made to look like arpabet, that we based of and people are familiar of
</commit_message>
<xml_diff>
--- a/SPREADSHEETS/BRAPA.xlsx
+++ b/SPREADSHEETS/BRAPA.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="BRAPA (PTBR)" sheetId="1" state="visible" r:id="rId3"/>
@@ -95,7 +95,7 @@
     <t xml:space="preserve">Regional (4 &amp; 9)</t>
   </si>
   <si>
-    <t xml:space="preserve">oa</t>
+    <t xml:space="preserve">ao</t>
   </si>
   <si>
     <t xml:space="preserve">(4) P"ó"rta - (9) Pedest"a"l</t>
@@ -120,7 +120,7 @@
         <family val="2"/>
         <charset val="128"/>
       </rPr>
-      <t xml:space="preserve">oa</t>
+      <t xml:space="preserve">ao</t>
     </r>
     <r>
       <rPr>
@@ -141,7 +141,7 @@
         <family val="2"/>
         <charset val="128"/>
       </rPr>
-      <t xml:space="preserve">oa</t>
+      <t xml:space="preserve">ao</t>
     </r>
     <r>
       <rPr>
@@ -2803,149 +2803,157 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -3133,1085 +3141,1085 @@
   </sheetPr>
   <dimension ref="B1:N77"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="37.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="27.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="35.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="19.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="37.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="27.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="35.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="19.33"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="1"/>
+      <c r="B1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="33.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="H6" s="6" t="s">
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="H6" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="8" t="s">
+      <c r="C7" s="8"/>
+      <c r="D7" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="12"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="12" t="s">
+      <c r="C8" s="14"/>
+      <c r="D8" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="14" t="s">
+      <c r="H8" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="12"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="16" t="s">
+      <c r="H9" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="12"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="H10" s="18" t="s">
+      <c r="H10" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="12"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="H11" s="19"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="11"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="12"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="12" t="n">
+      <c r="B12" s="13" t="n">
         <v>6</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="12" t="s">
+      <c r="C12" s="9"/>
+      <c r="D12" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="E12" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="12" t="s">
+      <c r="F12" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="H12" s="19"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="11"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="12"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="12" t="s">
+      <c r="C13" s="9"/>
+      <c r="D13" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="F13" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="H13" s="20"/>
-      <c r="I13" s="21"/>
-      <c r="J13" s="21"/>
-      <c r="K13" s="21"/>
-      <c r="L13" s="21"/>
-      <c r="M13" s="21"/>
-      <c r="N13" s="22"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="22"/>
+      <c r="L13" s="22"/>
+      <c r="M13" s="22"/>
+      <c r="N13" s="23"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="12" t="s">
+      <c r="C14" s="9"/>
+      <c r="D14" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="E14" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F14" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="H14" s="23" t="s">
+      <c r="H14" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="I14" s="23"/>
-      <c r="J14" s="23"/>
-      <c r="K14" s="23"/>
-      <c r="L14" s="23"/>
-      <c r="M14" s="23"/>
-      <c r="N14" s="23"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="24"/>
+      <c r="L14" s="24"/>
+      <c r="M14" s="24"/>
+      <c r="N14" s="24"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="12" t="s">
+      <c r="C15" s="9"/>
+      <c r="D15" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="E15" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="F15" s="12" t="s">
+      <c r="F15" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="H15" s="24"/>
-      <c r="I15" s="25"/>
-      <c r="J15" s="25"/>
-      <c r="K15" s="25"/>
-      <c r="L15" s="25"/>
-      <c r="M15" s="25"/>
-      <c r="N15" s="11"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="26"/>
+      <c r="M15" s="26"/>
+      <c r="N15" s="12"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="12" t="s">
+      <c r="C16" s="9"/>
+      <c r="D16" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E16" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="F16" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="H16" s="26" t="s">
+      <c r="H16" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
-      <c r="K16" s="26"/>
-      <c r="L16" s="26"/>
-      <c r="M16" s="26"/>
-      <c r="N16" s="26"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="27"/>
+      <c r="N16" s="27"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="27" t="s">
+      <c r="C17" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="E17" s="12" t="s">
+      <c r="E17" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="F17" s="12" t="s">
+      <c r="F17" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="H17" s="26" t="s">
+      <c r="H17" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26"/>
-      <c r="K17" s="26"/>
-      <c r="L17" s="26"/>
-      <c r="M17" s="26"/>
-      <c r="N17" s="26"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="27"/>
+      <c r="M17" s="27"/>
+      <c r="N17" s="27"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="12" t="s">
+      <c r="C18" s="9"/>
+      <c r="D18" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="E18" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="F18" s="12" t="s">
+      <c r="F18" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="H18" s="24"/>
-      <c r="I18" s="25"/>
-      <c r="J18" s="25"/>
-      <c r="K18" s="25"/>
-      <c r="L18" s="25"/>
-      <c r="M18" s="25"/>
-      <c r="N18" s="11"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
+      <c r="K18" s="26"/>
+      <c r="L18" s="26"/>
+      <c r="M18" s="26"/>
+      <c r="N18" s="12"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D19" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="E19" s="12" t="s">
+      <c r="E19" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="F19" s="12" t="s">
+      <c r="F19" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="H19" s="28" t="s">
+      <c r="H19" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="I19" s="28"/>
-      <c r="J19" s="28"/>
-      <c r="K19" s="28"/>
-      <c r="L19" s="28"/>
-      <c r="M19" s="28"/>
-      <c r="N19" s="28"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="29"/>
+      <c r="K19" s="29"/>
+      <c r="L19" s="29"/>
+      <c r="M19" s="29"/>
+      <c r="N19" s="29"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="12" t="s">
+      <c r="C20" s="9"/>
+      <c r="D20" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="E20" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="F20" s="12" t="s">
+      <c r="F20" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="H20" s="29" t="s">
+      <c r="H20" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="I20" s="29"/>
-      <c r="J20" s="29"/>
-      <c r="K20" s="29"/>
-      <c r="L20" s="29"/>
-      <c r="M20" s="29"/>
-      <c r="N20" s="29"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
+      <c r="K20" s="30"/>
+      <c r="L20" s="30"/>
+      <c r="M20" s="30"/>
+      <c r="N20" s="30"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="C21" s="8"/>
-      <c r="D21" s="12" t="s">
+      <c r="C21" s="9"/>
+      <c r="D21" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="E21" s="12" t="s">
+      <c r="E21" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="F21" s="12" t="s">
+      <c r="F21" s="13" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="C22" s="30" t="s">
+      <c r="C22" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="D22" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="E22" s="12" t="s">
+      <c r="E22" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="F22" s="12" t="s">
+      <c r="F22" s="13" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="12" t="s">
+      <c r="C23" s="9"/>
+      <c r="D23" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="E23" s="12" t="s">
+      <c r="E23" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="F23" s="12" t="s">
+      <c r="F23" s="13" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="C24" s="8"/>
-      <c r="D24" s="12" t="s">
+      <c r="C24" s="9"/>
+      <c r="D24" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="E24" s="12" t="s">
+      <c r="E24" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="F24" s="12" t="s">
+      <c r="F24" s="13" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="12" t="s">
+      <c r="B25" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="C25" s="8"/>
-      <c r="D25" s="12" t="s">
+      <c r="C25" s="9"/>
+      <c r="D25" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="E25" s="12" t="s">
+      <c r="E25" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="F25" s="12" t="s">
+      <c r="F25" s="13" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="12" t="s">
+      <c r="B26" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="C26" s="8"/>
-      <c r="D26" s="12" t="s">
+      <c r="C26" s="9"/>
+      <c r="D26" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="E26" s="12" t="s">
+      <c r="E26" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="F26" s="12" t="s">
+      <c r="F26" s="13" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="12" t="s">
+      <c r="B27" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="C27" s="8"/>
-      <c r="D27" s="12" t="s">
+      <c r="C27" s="9"/>
+      <c r="D27" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="E27" s="12" t="s">
+      <c r="E27" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="F27" s="12" t="s">
+      <c r="F27" s="13" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="12" t="s">
+      <c r="B28" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="C28" s="8"/>
-      <c r="D28" s="12" t="s">
+      <c r="C28" s="9"/>
+      <c r="D28" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="E28" s="12" t="s">
+      <c r="E28" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="F28" s="12" t="s">
+      <c r="F28" s="13" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="12" t="s">
+      <c r="B29" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="C29" s="31" t="s">
+      <c r="C29" s="32" t="s">
         <v>101</v>
       </c>
-      <c r="D29" s="12" t="s">
+      <c r="D29" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="E29" s="12" t="s">
+      <c r="E29" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="F29" s="12" t="s">
+      <c r="F29" s="13" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="C30" s="15" t="s">
+      <c r="C30" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="D30" s="12" t="s">
+      <c r="D30" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="E30" s="12" t="s">
+      <c r="E30" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="F30" s="12" t="s">
+      <c r="F30" s="13" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="32" t="s">
+      <c r="B32" s="33" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="33.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="33" t="s">
+      <c r="B38" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="C38" s="33"/>
-      <c r="D38" s="33"/>
-      <c r="E38" s="33"/>
-      <c r="F38" s="33"/>
+      <c r="C38" s="34"/>
+      <c r="D38" s="34"/>
+      <c r="E38" s="34"/>
+      <c r="F38" s="34"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="7" t="s">
+      <c r="B39" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C39" s="7"/>
-      <c r="D39" s="8" t="s">
+      <c r="C39" s="8"/>
+      <c r="D39" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="E39" s="8" t="s">
+      <c r="E39" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F39" s="8" t="s">
+      <c r="F39" s="9" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="12" t="s">
+      <c r="B40" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="C40" s="13"/>
-      <c r="D40" s="12" t="s">
+      <c r="C40" s="14"/>
+      <c r="D40" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="E40" s="12" t="s">
+      <c r="E40" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="F40" s="12" t="s">
+      <c r="F40" s="13" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="12" t="s">
+      <c r="B41" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="C41" s="15"/>
-      <c r="D41" s="12" t="s">
+      <c r="C41" s="16"/>
+      <c r="D41" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="E41" s="12" t="s">
+      <c r="E41" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="F41" s="12" t="s">
+      <c r="F41" s="13" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="33.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="34" t="s">
+      <c r="B47" s="35" t="s">
         <v>119</v>
       </c>
-      <c r="C47" s="34"/>
-      <c r="D47" s="34"/>
-      <c r="E47" s="34"/>
-      <c r="F47" s="34"/>
+      <c r="C47" s="35"/>
+      <c r="D47" s="35"/>
+      <c r="E47" s="35"/>
+      <c r="F47" s="35"/>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="7" t="s">
+      <c r="B48" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C48" s="7"/>
-      <c r="D48" s="8" t="s">
+      <c r="C48" s="8"/>
+      <c r="D48" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="E48" s="8" t="s">
+      <c r="E48" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F48" s="8" t="s">
+      <c r="F48" s="9" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="12" t="s">
+      <c r="B49" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="C49" s="8"/>
-      <c r="D49" s="12" t="s">
+      <c r="C49" s="9"/>
+      <c r="D49" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="E49" s="12" t="s">
+      <c r="E49" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="F49" s="12" t="s">
+      <c r="F49" s="13" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="12" t="s">
+      <c r="B50" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="C50" s="15"/>
-      <c r="D50" s="12" t="s">
+      <c r="C50" s="16"/>
+      <c r="D50" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="E50" s="12" t="s">
+      <c r="E50" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="F50" s="12" t="s">
+      <c r="F50" s="13" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="12" t="s">
+      <c r="B51" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="C51" s="8"/>
-      <c r="D51" s="12" t="s">
+      <c r="C51" s="9"/>
+      <c r="D51" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="E51" s="12" t="s">
+      <c r="E51" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="F51" s="8" t="s">
+      <c r="F51" s="9" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="12" t="s">
+      <c r="B52" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="C52" s="8"/>
-      <c r="D52" s="12" t="s">
+      <c r="C52" s="9"/>
+      <c r="D52" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="E52" s="12" t="s">
+      <c r="E52" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="F52" s="12" t="s">
+      <c r="F52" s="13" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="12" t="s">
+      <c r="B53" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="C53" s="8"/>
-      <c r="D53" s="12" t="s">
+      <c r="C53" s="9"/>
+      <c r="D53" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="E53" s="12" t="s">
+      <c r="E53" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="F53" s="12" t="s">
+      <c r="F53" s="13" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B54" s="12" t="s">
+      <c r="B54" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="C54" s="8"/>
-      <c r="D54" s="12" t="s">
+      <c r="C54" s="9"/>
+      <c r="D54" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="E54" s="12" t="s">
+      <c r="E54" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="F54" s="12" t="s">
+      <c r="F54" s="13" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="12" t="s">
+      <c r="B55" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="C55" s="8"/>
-      <c r="D55" s="12" t="s">
+      <c r="C55" s="9"/>
+      <c r="D55" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="E55" s="12" t="s">
+      <c r="E55" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="F55" s="12" t="s">
+      <c r="F55" s="13" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="12" t="s">
+      <c r="B56" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="C56" s="8"/>
-      <c r="D56" s="12" t="s">
+      <c r="C56" s="9"/>
+      <c r="D56" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="E56" s="12" t="s">
+      <c r="E56" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="F56" s="12" t="s">
+      <c r="F56" s="13" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="12" t="s">
+      <c r="B57" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="C57" s="8"/>
-      <c r="D57" s="12" t="s">
+      <c r="C57" s="9"/>
+      <c r="D57" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="E57" s="12" t="s">
+      <c r="E57" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="F57" s="12" t="s">
+      <c r="F57" s="13" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="12" t="s">
+      <c r="B58" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="C58" s="8"/>
-      <c r="D58" s="12" t="s">
+      <c r="C58" s="9"/>
+      <c r="D58" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="E58" s="12" t="s">
+      <c r="E58" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="F58" s="12" t="s">
+      <c r="F58" s="13" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="8" t="n">
+      <c r="B59" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="C59" s="8"/>
-      <c r="D59" s="12" t="s">
+      <c r="C59" s="9"/>
+      <c r="D59" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="E59" s="12" t="s">
+      <c r="E59" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="F59" s="12" t="s">
+      <c r="F59" s="13" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="12" t="s">
+      <c r="B60" s="13" t="s">
         <v>157</v>
       </c>
-      <c r="C60" s="8"/>
-      <c r="D60" s="12" t="s">
+      <c r="C60" s="9"/>
+      <c r="D60" s="13" t="s">
         <v>157</v>
       </c>
-      <c r="E60" s="12" t="s">
+      <c r="E60" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="F60" s="12" t="s">
+      <c r="F60" s="13" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="12" t="s">
+      <c r="B61" s="13" t="s">
         <v>160</v>
       </c>
-      <c r="C61" s="8"/>
-      <c r="D61" s="12" t="s">
+      <c r="C61" s="9"/>
+      <c r="D61" s="13" t="s">
         <v>160</v>
       </c>
-      <c r="E61" s="12" t="s">
+      <c r="E61" s="13" t="s">
         <v>161</v>
       </c>
-      <c r="F61" s="12" t="s">
+      <c r="F61" s="13" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="12" t="s">
+      <c r="B62" s="13" t="s">
         <v>163</v>
       </c>
-      <c r="C62" s="8"/>
-      <c r="D62" s="12" t="s">
+      <c r="C62" s="9"/>
+      <c r="D62" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="E62" s="12" t="s">
+      <c r="E62" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="F62" s="12" t="s">
+      <c r="F62" s="13" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B63" s="12" t="s">
+      <c r="B63" s="13" t="s">
         <v>167</v>
       </c>
-      <c r="C63" s="8"/>
-      <c r="D63" s="12" t="s">
+      <c r="C63" s="9"/>
+      <c r="D63" s="13" t="s">
         <v>168</v>
       </c>
-      <c r="E63" s="12" t="s">
+      <c r="E63" s="13" t="s">
         <v>169</v>
       </c>
-      <c r="F63" s="12" t="s">
+      <c r="F63" s="13" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B64" s="12" t="s">
+      <c r="B64" s="13" t="s">
         <v>171</v>
       </c>
-      <c r="C64" s="8"/>
-      <c r="D64" s="12" t="s">
+      <c r="C64" s="9"/>
+      <c r="D64" s="13" t="s">
         <v>171</v>
       </c>
-      <c r="E64" s="12" t="s">
+      <c r="E64" s="13" t="s">
         <v>172</v>
       </c>
-      <c r="F64" s="12" t="s">
+      <c r="F64" s="13" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B65" s="12" t="s">
+      <c r="B65" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="C65" s="35" t="s">
+      <c r="C65" s="36" t="s">
         <v>175</v>
       </c>
-      <c r="D65" s="12" t="s">
+      <c r="D65" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="E65" s="12" t="s">
+      <c r="E65" s="13" t="s">
         <v>177</v>
       </c>
-      <c r="F65" s="12" t="s">
+      <c r="F65" s="13" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B66" s="12" t="s">
+      <c r="B66" s="13" t="s">
         <v>179</v>
       </c>
-      <c r="C66" s="35" t="s">
+      <c r="C66" s="36" t="s">
         <v>175</v>
       </c>
-      <c r="D66" s="12" t="s">
+      <c r="D66" s="13" t="s">
         <v>180</v>
       </c>
-      <c r="E66" s="12" t="s">
+      <c r="E66" s="13" t="s">
         <v>181</v>
       </c>
-      <c r="F66" s="12" t="s">
+      <c r="F66" s="13" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B67" s="8" t="n">
+      <c r="B67" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="C67" s="8"/>
-      <c r="D67" s="12" t="s">
+      <c r="C67" s="9"/>
+      <c r="D67" s="13" t="s">
         <v>183</v>
       </c>
-      <c r="E67" s="12" t="s">
+      <c r="E67" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="F67" s="12" t="s">
+      <c r="F67" s="13" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B68" s="12" t="s">
+      <c r="B68" s="13" t="s">
         <v>183</v>
       </c>
-      <c r="C68" s="35" t="s">
+      <c r="C68" s="36" t="s">
         <v>175</v>
       </c>
-      <c r="D68" s="12" t="s">
+      <c r="D68" s="13" t="s">
         <v>186</v>
       </c>
-      <c r="E68" s="12" t="s">
+      <c r="E68" s="13" t="s">
         <v>187</v>
       </c>
-      <c r="F68" s="12" t="s">
+      <c r="F68" s="13" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B69" s="12" t="s">
+      <c r="B69" s="13" t="s">
         <v>189</v>
       </c>
-      <c r="C69" s="8"/>
-      <c r="D69" s="12" t="s">
+      <c r="C69" s="9"/>
+      <c r="D69" s="13" t="s">
         <v>189</v>
       </c>
-      <c r="E69" s="12" t="s">
+      <c r="E69" s="13" t="s">
         <v>190</v>
       </c>
-      <c r="F69" s="12" t="s">
+      <c r="F69" s="13" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B70" s="12" t="s">
+      <c r="B70" s="13" t="s">
         <v>192</v>
       </c>
-      <c r="C70" s="8"/>
-      <c r="D70" s="12" t="s">
+      <c r="C70" s="9"/>
+      <c r="D70" s="13" t="s">
         <v>192</v>
       </c>
-      <c r="E70" s="12" t="s">
+      <c r="E70" s="13" t="s">
         <v>193</v>
       </c>
-      <c r="F70" s="12" t="s">
+      <c r="F70" s="13" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B71" s="12" t="s">
+      <c r="B71" s="13" t="s">
         <v>195</v>
       </c>
-      <c r="C71" s="8"/>
-      <c r="D71" s="12" t="s">
+      <c r="C71" s="9"/>
+      <c r="D71" s="13" t="s">
         <v>196</v>
       </c>
-      <c r="E71" s="12" t="s">
+      <c r="E71" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="F71" s="12" t="s">
+      <c r="F71" s="13" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B72" s="12" t="s">
+      <c r="B72" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="C72" s="8"/>
-      <c r="D72" s="12" t="s">
+      <c r="C72" s="9"/>
+      <c r="D72" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="E72" s="12" t="s">
+      <c r="E72" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="F72" s="12" t="s">
+      <c r="F72" s="13" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B73" s="12" t="s">
+      <c r="B73" s="13" t="s">
         <v>202</v>
       </c>
-      <c r="C73" s="8"/>
-      <c r="D73" s="12" t="s">
+      <c r="C73" s="9"/>
+      <c r="D73" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="E73" s="12" t="s">
+      <c r="E73" s="13" t="s">
         <v>204</v>
       </c>
-      <c r="F73" s="12" t="s">
+      <c r="F73" s="13" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B74" s="12" t="s">
+      <c r="B74" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="C74" s="8"/>
-      <c r="D74" s="12" t="s">
+      <c r="C74" s="9"/>
+      <c r="D74" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="E74" s="12" t="s">
+      <c r="E74" s="13" t="s">
         <v>207</v>
       </c>
-      <c r="F74" s="12" t="s">
+      <c r="F74" s="13" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B75" s="12" t="s">
+      <c r="B75" s="13" t="s">
         <v>209</v>
       </c>
-      <c r="C75" s="8"/>
-      <c r="D75" s="12" t="s">
+      <c r="C75" s="9"/>
+      <c r="D75" s="13" t="s">
         <v>209</v>
       </c>
-      <c r="E75" s="12" t="s">
+      <c r="E75" s="13" t="s">
         <v>210</v>
       </c>
-      <c r="F75" s="12" t="s">
+      <c r="F75" s="13" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B76" s="12" t="s">
+      <c r="B76" s="13" t="s">
         <v>212</v>
       </c>
-      <c r="C76" s="8"/>
-      <c r="D76" s="12" t="s">
+      <c r="C76" s="9"/>
+      <c r="D76" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="E76" s="12" t="s">
+      <c r="E76" s="13" t="s">
         <v>213</v>
       </c>
-      <c r="F76" s="12" t="s">
+      <c r="F76" s="13" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B77" s="12" t="s">
+      <c r="B77" s="13" t="s">
         <v>215</v>
       </c>
-      <c r="C77" s="8"/>
-      <c r="D77" s="12" t="s">
+      <c r="C77" s="9"/>
+      <c r="D77" s="13" t="s">
         <v>215</v>
       </c>
-      <c r="E77" s="12" t="s">
+      <c r="E77" s="13" t="s">
         <v>216</v>
       </c>
-      <c r="F77" s="12" t="s">
+      <c r="F77" s="13" t="s">
         <v>217</v>
       </c>
     </row>
@@ -4252,1089 +4260,1089 @@
   </sheetPr>
   <dimension ref="B1:N77"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="37.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="27.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="35.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="19.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="37.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="27.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="35.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="19.33"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="1"/>
+      <c r="B1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="33.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="H6" s="6" t="s">
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="H6" s="7" t="s">
         <v>219</v>
       </c>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="8" t="s">
+      <c r="C7" s="8"/>
+      <c r="D7" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="9" t="s">
         <v>221</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="12"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="12" t="s">
+      <c r="C8" s="14"/>
+      <c r="D8" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="14" t="s">
+      <c r="H8" s="15" t="s">
         <v>222</v>
       </c>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="12"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="16" t="s">
+      <c r="H9" s="17" t="s">
         <v>223</v>
       </c>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="12"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="18" t="s">
         <v>224</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="H10" s="18" t="s">
+      <c r="H10" s="19" t="s">
         <v>225</v>
       </c>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="12"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="H11" s="19"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="11"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="12"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="12" t="n">
+      <c r="B12" s="13" t="n">
         <v>6</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="12" t="s">
+      <c r="C12" s="9"/>
+      <c r="D12" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="E12" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="12" t="s">
+      <c r="F12" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="H12" s="19"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="11"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="12"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="12" t="s">
+      <c r="C13" s="9"/>
+      <c r="D13" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="F13" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="H13" s="20"/>
-      <c r="I13" s="21"/>
-      <c r="J13" s="21"/>
-      <c r="K13" s="21"/>
-      <c r="L13" s="21"/>
-      <c r="M13" s="21"/>
-      <c r="N13" s="22"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="22"/>
+      <c r="L13" s="22"/>
+      <c r="M13" s="22"/>
+      <c r="N13" s="23"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="12" t="s">
+      <c r="C14" s="9"/>
+      <c r="D14" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="E14" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F14" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="H14" s="23" t="s">
+      <c r="H14" s="24" t="s">
         <v>226</v>
       </c>
-      <c r="I14" s="23"/>
-      <c r="J14" s="23"/>
-      <c r="K14" s="23"/>
-      <c r="L14" s="23"/>
-      <c r="M14" s="23"/>
-      <c r="N14" s="23"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="24"/>
+      <c r="L14" s="24"/>
+      <c r="M14" s="24"/>
+      <c r="N14" s="24"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="12" t="s">
+      <c r="C15" s="9"/>
+      <c r="D15" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="E15" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="F15" s="12" t="s">
+      <c r="F15" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="H15" s="24"/>
-      <c r="I15" s="25"/>
-      <c r="J15" s="25"/>
-      <c r="K15" s="25"/>
-      <c r="L15" s="25"/>
-      <c r="M15" s="25"/>
-      <c r="N15" s="11"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="26"/>
+      <c r="M15" s="26"/>
+      <c r="N15" s="12"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="12" t="s">
+      <c r="C16" s="9"/>
+      <c r="D16" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E16" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="F16" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="H16" s="26" t="s">
+      <c r="H16" s="27" t="s">
         <v>227</v>
       </c>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
-      <c r="K16" s="26"/>
-      <c r="L16" s="26"/>
-      <c r="M16" s="26"/>
-      <c r="N16" s="26"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="27"/>
+      <c r="N16" s="27"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="27" t="s">
+      <c r="C17" s="28" t="s">
         <v>228</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="E17" s="12" t="s">
+      <c r="E17" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="F17" s="12" t="s">
+      <c r="F17" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="H17" s="26" t="s">
+      <c r="H17" s="27" t="s">
         <v>229</v>
       </c>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26"/>
-      <c r="K17" s="26"/>
-      <c r="L17" s="26"/>
-      <c r="M17" s="26"/>
-      <c r="N17" s="26"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="27"/>
+      <c r="M17" s="27"/>
+      <c r="N17" s="27"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="12" t="s">
+      <c r="C18" s="9"/>
+      <c r="D18" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="E18" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="F18" s="12" t="s">
+      <c r="F18" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="H18" s="24"/>
-      <c r="I18" s="25"/>
-      <c r="J18" s="25"/>
-      <c r="K18" s="25"/>
-      <c r="L18" s="25"/>
-      <c r="M18" s="25"/>
-      <c r="N18" s="11"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
+      <c r="K18" s="26"/>
+      <c r="L18" s="26"/>
+      <c r="M18" s="26"/>
+      <c r="N18" s="12"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D19" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="E19" s="12" t="s">
+      <c r="E19" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="F19" s="12" t="s">
+      <c r="F19" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="H19" s="28" t="s">
+      <c r="H19" s="29" t="s">
         <v>230</v>
       </c>
-      <c r="I19" s="28"/>
-      <c r="J19" s="28"/>
-      <c r="K19" s="28"/>
-      <c r="L19" s="28"/>
-      <c r="M19" s="28"/>
-      <c r="N19" s="28"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="29"/>
+      <c r="K19" s="29"/>
+      <c r="L19" s="29"/>
+      <c r="M19" s="29"/>
+      <c r="N19" s="29"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="12" t="s">
+      <c r="C20" s="9"/>
+      <c r="D20" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="E20" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="F20" s="12" t="s">
+      <c r="F20" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="H20" s="29" t="s">
+      <c r="H20" s="30" t="s">
         <v>231</v>
       </c>
-      <c r="I20" s="29"/>
-      <c r="J20" s="29"/>
-      <c r="K20" s="29"/>
-      <c r="L20" s="29"/>
-      <c r="M20" s="29"/>
-      <c r="N20" s="29"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
+      <c r="K20" s="30"/>
+      <c r="L20" s="30"/>
+      <c r="M20" s="30"/>
+      <c r="N20" s="30"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="C21" s="8"/>
-      <c r="D21" s="12" t="s">
+      <c r="C21" s="9"/>
+      <c r="D21" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="E21" s="12" t="s">
+      <c r="E21" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="F21" s="12" t="s">
+      <c r="F21" s="13" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="C22" s="30" t="s">
+      <c r="C22" s="31" t="s">
         <v>232</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="D22" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="E22" s="12" t="s">
+      <c r="E22" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="F22" s="12" t="s">
+      <c r="F22" s="13" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="12" t="s">
+      <c r="C23" s="9"/>
+      <c r="D23" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="E23" s="12" t="s">
+      <c r="E23" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="F23" s="12" t="s">
+      <c r="F23" s="13" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="C24" s="8"/>
-      <c r="D24" s="12" t="s">
+      <c r="C24" s="9"/>
+      <c r="D24" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="E24" s="12" t="s">
+      <c r="E24" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="F24" s="12" t="s">
+      <c r="F24" s="13" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="12" t="s">
+      <c r="B25" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="C25" s="8"/>
-      <c r="D25" s="12" t="s">
+      <c r="C25" s="9"/>
+      <c r="D25" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="E25" s="12" t="s">
+      <c r="E25" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="F25" s="12" t="s">
+      <c r="F25" s="13" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="12" t="s">
+      <c r="B26" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="C26" s="8"/>
-      <c r="D26" s="12" t="s">
+      <c r="C26" s="9"/>
+      <c r="D26" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="E26" s="12" t="s">
+      <c r="E26" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="F26" s="12" t="s">
+      <c r="F26" s="13" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="12" t="s">
+      <c r="B27" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="C27" s="8"/>
-      <c r="D27" s="12" t="s">
+      <c r="C27" s="9"/>
+      <c r="D27" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="E27" s="12" t="s">
+      <c r="E27" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="F27" s="12" t="s">
+      <c r="F27" s="13" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="12" t="s">
+      <c r="B28" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="C28" s="8"/>
-      <c r="D28" s="12" t="s">
+      <c r="C28" s="9"/>
+      <c r="D28" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="E28" s="12" t="s">
+      <c r="E28" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="F28" s="12" t="s">
+      <c r="F28" s="13" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="12" t="s">
+      <c r="B29" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="C29" s="31" t="s">
+      <c r="C29" s="32" t="s">
         <v>233</v>
       </c>
-      <c r="D29" s="12" t="s">
+      <c r="D29" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="E29" s="12" t="s">
+      <c r="E29" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="F29" s="12" t="s">
+      <c r="F29" s="13" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="C30" s="15" t="s">
+      <c r="C30" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="D30" s="12" t="s">
+      <c r="D30" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="E30" s="12" t="s">
+      <c r="E30" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="F30" s="12" t="s">
+      <c r="F30" s="13" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="32" t="s">
+      <c r="B32" s="37" t="s">
         <v>234</v>
       </c>
-      <c r="C32" s="32"/>
-      <c r="D32" s="32"/>
-      <c r="E32" s="32"/>
-      <c r="F32" s="32"/>
+      <c r="C32" s="37"/>
+      <c r="D32" s="37"/>
+      <c r="E32" s="37"/>
+      <c r="F32" s="37"/>
     </row>
     <row r="38" customFormat="false" ht="33.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="33" t="s">
+      <c r="B38" s="34" t="s">
         <v>235</v>
       </c>
-      <c r="C38" s="33"/>
-      <c r="D38" s="33"/>
-      <c r="E38" s="33"/>
-      <c r="F38" s="33"/>
+      <c r="C38" s="34"/>
+      <c r="D38" s="34"/>
+      <c r="E38" s="34"/>
+      <c r="F38" s="34"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="7" t="s">
+      <c r="B39" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C39" s="7"/>
-      <c r="D39" s="8" t="s">
+      <c r="C39" s="8"/>
+      <c r="D39" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="E39" s="8" t="s">
+      <c r="E39" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="F39" s="8" t="s">
+      <c r="F39" s="9" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="12" t="s">
+      <c r="B40" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="C40" s="13"/>
-      <c r="D40" s="12" t="s">
+      <c r="C40" s="14"/>
+      <c r="D40" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="E40" s="12" t="s">
+      <c r="E40" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="F40" s="12" t="s">
+      <c r="F40" s="13" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="12" t="s">
+      <c r="B41" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="C41" s="15"/>
-      <c r="D41" s="12" t="s">
+      <c r="C41" s="16"/>
+      <c r="D41" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="E41" s="12" t="s">
+      <c r="E41" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="F41" s="12" t="s">
+      <c r="F41" s="13" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="33.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="34" t="s">
+      <c r="B47" s="35" t="s">
         <v>236</v>
       </c>
-      <c r="C47" s="34"/>
-      <c r="D47" s="34"/>
-      <c r="E47" s="34"/>
-      <c r="F47" s="34"/>
+      <c r="C47" s="35"/>
+      <c r="D47" s="35"/>
+      <c r="E47" s="35"/>
+      <c r="F47" s="35"/>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="7" t="s">
+      <c r="B48" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C48" s="7"/>
-      <c r="D48" s="8" t="s">
+      <c r="C48" s="8"/>
+      <c r="D48" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="E48" s="8" t="s">
+      <c r="E48" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="F48" s="8" t="s">
+      <c r="F48" s="9" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="12" t="s">
+      <c r="B49" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="C49" s="8"/>
-      <c r="D49" s="12" t="s">
+      <c r="C49" s="9"/>
+      <c r="D49" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="E49" s="12" t="s">
+      <c r="E49" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="F49" s="12" t="s">
+      <c r="F49" s="13" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="12" t="s">
+      <c r="B50" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="C50" s="15"/>
-      <c r="D50" s="12" t="s">
+      <c r="C50" s="16"/>
+      <c r="D50" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="E50" s="12" t="s">
+      <c r="E50" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="F50" s="12" t="s">
+      <c r="F50" s="13" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="12" t="s">
+      <c r="B51" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="C51" s="8"/>
-      <c r="D51" s="12" t="s">
+      <c r="C51" s="9"/>
+      <c r="D51" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="E51" s="12" t="s">
+      <c r="E51" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="F51" s="8" t="s">
+      <c r="F51" s="9" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="12" t="s">
+      <c r="B52" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="C52" s="8"/>
-      <c r="D52" s="12" t="s">
+      <c r="C52" s="9"/>
+      <c r="D52" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="E52" s="12" t="s">
+      <c r="E52" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="F52" s="12" t="s">
+      <c r="F52" s="13" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="12" t="s">
+      <c r="B53" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="C53" s="8"/>
-      <c r="D53" s="12" t="s">
+      <c r="C53" s="9"/>
+      <c r="D53" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="E53" s="12" t="s">
+      <c r="E53" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="F53" s="12" t="s">
+      <c r="F53" s="13" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B54" s="12" t="s">
+      <c r="B54" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="C54" s="8"/>
-      <c r="D54" s="12" t="s">
+      <c r="C54" s="9"/>
+      <c r="D54" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="E54" s="12" t="s">
+      <c r="E54" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="F54" s="12" t="s">
+      <c r="F54" s="13" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="12" t="s">
+      <c r="B55" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="C55" s="8"/>
-      <c r="D55" s="12" t="s">
+      <c r="C55" s="9"/>
+      <c r="D55" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="E55" s="12" t="s">
+      <c r="E55" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="F55" s="12" t="s">
+      <c r="F55" s="13" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="12" t="s">
+      <c r="B56" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="C56" s="8"/>
-      <c r="D56" s="12" t="s">
+      <c r="C56" s="9"/>
+      <c r="D56" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="E56" s="12" t="s">
+      <c r="E56" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="F56" s="12" t="s">
+      <c r="F56" s="13" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="12" t="s">
+      <c r="B57" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="C57" s="8"/>
-      <c r="D57" s="12" t="s">
+      <c r="C57" s="9"/>
+      <c r="D57" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="E57" s="12" t="s">
+      <c r="E57" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="F57" s="12" t="s">
+      <c r="F57" s="13" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="12" t="s">
+      <c r="B58" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="C58" s="8"/>
-      <c r="D58" s="12" t="s">
+      <c r="C58" s="9"/>
+      <c r="D58" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="E58" s="12" t="s">
+      <c r="E58" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="F58" s="12" t="s">
+      <c r="F58" s="13" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="8" t="n">
+      <c r="B59" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="C59" s="8"/>
-      <c r="D59" s="12" t="s">
+      <c r="C59" s="9"/>
+      <c r="D59" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="E59" s="12" t="s">
+      <c r="E59" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="F59" s="12" t="s">
+      <c r="F59" s="13" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="12" t="s">
+      <c r="B60" s="13" t="s">
         <v>157</v>
       </c>
-      <c r="C60" s="8"/>
-      <c r="D60" s="12" t="s">
+      <c r="C60" s="9"/>
+      <c r="D60" s="13" t="s">
         <v>157</v>
       </c>
-      <c r="E60" s="12" t="s">
+      <c r="E60" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="F60" s="12" t="s">
+      <c r="F60" s="13" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="12" t="s">
+      <c r="B61" s="13" t="s">
         <v>160</v>
       </c>
-      <c r="C61" s="8"/>
-      <c r="D61" s="12" t="s">
+      <c r="C61" s="9"/>
+      <c r="D61" s="13" t="s">
         <v>160</v>
       </c>
-      <c r="E61" s="12" t="s">
+      <c r="E61" s="13" t="s">
         <v>161</v>
       </c>
-      <c r="F61" s="12" t="s">
+      <c r="F61" s="13" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="12" t="s">
+      <c r="B62" s="13" t="s">
         <v>163</v>
       </c>
-      <c r="C62" s="8"/>
-      <c r="D62" s="12" t="s">
+      <c r="C62" s="9"/>
+      <c r="D62" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="E62" s="12" t="s">
+      <c r="E62" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="F62" s="12" t="s">
+      <c r="F62" s="13" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B63" s="12" t="s">
+      <c r="B63" s="13" t="s">
         <v>167</v>
       </c>
-      <c r="C63" s="8"/>
-      <c r="D63" s="12" t="s">
+      <c r="C63" s="9"/>
+      <c r="D63" s="13" t="s">
         <v>168</v>
       </c>
-      <c r="E63" s="12" t="s">
+      <c r="E63" s="13" t="s">
         <v>169</v>
       </c>
-      <c r="F63" s="12" t="s">
+      <c r="F63" s="13" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B64" s="12" t="s">
+      <c r="B64" s="13" t="s">
         <v>171</v>
       </c>
-      <c r="C64" s="8"/>
-      <c r="D64" s="12" t="s">
+      <c r="C64" s="9"/>
+      <c r="D64" s="13" t="s">
         <v>171</v>
       </c>
-      <c r="E64" s="12" t="s">
+      <c r="E64" s="13" t="s">
         <v>172</v>
       </c>
-      <c r="F64" s="12" t="s">
+      <c r="F64" s="13" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B65" s="12" t="s">
+      <c r="B65" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="C65" s="35" t="s">
+      <c r="C65" s="36" t="s">
         <v>175</v>
       </c>
-      <c r="D65" s="12" t="s">
+      <c r="D65" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="E65" s="12" t="s">
+      <c r="E65" s="13" t="s">
         <v>177</v>
       </c>
-      <c r="F65" s="12" t="s">
+      <c r="F65" s="13" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B66" s="12" t="s">
+      <c r="B66" s="13" t="s">
         <v>179</v>
       </c>
-      <c r="C66" s="35" t="s">
+      <c r="C66" s="36" t="s">
         <v>175</v>
       </c>
-      <c r="D66" s="12" t="s">
+      <c r="D66" s="13" t="s">
         <v>180</v>
       </c>
-      <c r="E66" s="12" t="s">
+      <c r="E66" s="13" t="s">
         <v>181</v>
       </c>
-      <c r="F66" s="12" t="s">
+      <c r="F66" s="13" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B67" s="8" t="n">
+      <c r="B67" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="C67" s="8"/>
-      <c r="D67" s="12" t="s">
+      <c r="C67" s="9"/>
+      <c r="D67" s="13" t="s">
         <v>183</v>
       </c>
-      <c r="E67" s="12" t="s">
+      <c r="E67" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="F67" s="12" t="s">
+      <c r="F67" s="13" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B68" s="12" t="s">
+      <c r="B68" s="13" t="s">
         <v>183</v>
       </c>
-      <c r="C68" s="35" t="s">
+      <c r="C68" s="36" t="s">
         <v>175</v>
       </c>
-      <c r="D68" s="12" t="s">
+      <c r="D68" s="13" t="s">
         <v>186</v>
       </c>
-      <c r="E68" s="12" t="s">
+      <c r="E68" s="13" t="s">
         <v>187</v>
       </c>
-      <c r="F68" s="12" t="s">
+      <c r="F68" s="13" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B69" s="12" t="s">
+      <c r="B69" s="13" t="s">
         <v>189</v>
       </c>
-      <c r="C69" s="8"/>
-      <c r="D69" s="12" t="s">
+      <c r="C69" s="9"/>
+      <c r="D69" s="13" t="s">
         <v>189</v>
       </c>
-      <c r="E69" s="12" t="s">
+      <c r="E69" s="13" t="s">
         <v>190</v>
       </c>
-      <c r="F69" s="12" t="s">
+      <c r="F69" s="13" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B70" s="12" t="s">
+      <c r="B70" s="13" t="s">
         <v>192</v>
       </c>
-      <c r="C70" s="8"/>
-      <c r="D70" s="12" t="s">
+      <c r="C70" s="9"/>
+      <c r="D70" s="13" t="s">
         <v>192</v>
       </c>
-      <c r="E70" s="12" t="s">
+      <c r="E70" s="13" t="s">
         <v>193</v>
       </c>
-      <c r="F70" s="12" t="s">
+      <c r="F70" s="13" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B71" s="12" t="s">
+      <c r="B71" s="13" t="s">
         <v>195</v>
       </c>
-      <c r="C71" s="8"/>
-      <c r="D71" s="12" t="s">
+      <c r="C71" s="9"/>
+      <c r="D71" s="13" t="s">
         <v>196</v>
       </c>
-      <c r="E71" s="12" t="s">
+      <c r="E71" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="F71" s="12" t="s">
+      <c r="F71" s="13" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B72" s="12" t="s">
+      <c r="B72" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="C72" s="8"/>
-      <c r="D72" s="12" t="s">
+      <c r="C72" s="9"/>
+      <c r="D72" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="E72" s="12" t="s">
+      <c r="E72" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="F72" s="12" t="s">
+      <c r="F72" s="13" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B73" s="12" t="s">
+      <c r="B73" s="13" t="s">
         <v>202</v>
       </c>
-      <c r="C73" s="8"/>
-      <c r="D73" s="12" t="s">
+      <c r="C73" s="9"/>
+      <c r="D73" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="E73" s="12" t="s">
+      <c r="E73" s="13" t="s">
         <v>204</v>
       </c>
-      <c r="F73" s="12" t="s">
+      <c r="F73" s="13" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B74" s="12" t="s">
+      <c r="B74" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="C74" s="8"/>
-      <c r="D74" s="12" t="s">
+      <c r="C74" s="9"/>
+      <c r="D74" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="E74" s="12" t="s">
+      <c r="E74" s="13" t="s">
         <v>207</v>
       </c>
-      <c r="F74" s="12" t="s">
+      <c r="F74" s="13" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B75" s="12" t="s">
+      <c r="B75" s="13" t="s">
         <v>209</v>
       </c>
-      <c r="C75" s="8"/>
-      <c r="D75" s="12" t="s">
+      <c r="C75" s="9"/>
+      <c r="D75" s="13" t="s">
         <v>209</v>
       </c>
-      <c r="E75" s="12" t="s">
+      <c r="E75" s="13" t="s">
         <v>210</v>
       </c>
-      <c r="F75" s="12" t="s">
+      <c r="F75" s="13" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B76" s="12" t="s">
+      <c r="B76" s="13" t="s">
         <v>212</v>
       </c>
-      <c r="C76" s="8"/>
-      <c r="D76" s="12" t="s">
+      <c r="C76" s="9"/>
+      <c r="D76" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="E76" s="12" t="s">
+      <c r="E76" s="13" t="s">
         <v>213</v>
       </c>
-      <c r="F76" s="12" t="s">
+      <c r="F76" s="13" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B77" s="12" t="s">
+      <c r="B77" s="13" t="s">
         <v>215</v>
       </c>
-      <c r="C77" s="8"/>
-      <c r="D77" s="12" t="s">
+      <c r="C77" s="9"/>
+      <c r="D77" s="13" t="s">
         <v>215</v>
       </c>
-      <c r="E77" s="12" t="s">
+      <c r="E77" s="13" t="s">
         <v>216</v>
       </c>
-      <c r="F77" s="12" t="s">
+      <c r="F77" s="13" t="s">
         <v>217</v>
       </c>
     </row>

</xml_diff>